<commit_message>
20250106 fix hp recover gimmick
</commit_message>
<xml_diff>
--- a/casual1/Assets/Resources/LevelDB.xlsx
+++ b/casual1/Assets/Resources/LevelDB.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,6 +86,10 @@
   </si>
   <si>
     <t>20301:130</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10501:180</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -415,7 +419,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -474,6 +478,9 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">

</xml_diff>

<commit_message>
20250106 change launcher position
</commit_message>
<xml_diff>
--- a/casual1/Assets/Resources/LevelDB.xlsx
+++ b/casual1/Assets/Resources/LevelDB.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,6 +90,14 @@
   </si>
   <si>
     <t>10501:180</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10102:0:45:90:135:180:225:270:315</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10102:0:45:90:135:225:270:315</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -419,12 +427,13 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="10" width="19.125" customWidth="1"/>
+    <col min="6" max="6" width="31.375" customWidth="1"/>
+    <col min="7" max="10" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -476,7 +485,7 @@
         <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
@@ -499,7 +508,7 @@
         <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
20250109 add art resources
</commit_message>
<xml_diff>
--- a/casual1/Assets/Resources/LevelDB.xlsx
+++ b/casual1/Assets/Resources/LevelDB.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,6 +98,10 @@
   </si>
   <si>
     <t>10102:0:45:90:135:225:270:315</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10801:250</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -427,7 +431,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -679,6 +683,9 @@
       <c r="G11" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>